<commit_message>
Complete los entregables de la columna Franco
</commit_message>
<xml_diff>
--- a/Documento de consistencia.xlsx
+++ b/Documento de consistencia.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Documentos</t>
   </si>
@@ -150,6 +150,21 @@
   <si>
     <t>A revisar por:</t>
   </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>si(lo tengo que sacar)</t>
+  </si>
+  <si>
+    <t>si(tambien tengo gestion de riesgos)</t>
+  </si>
+  <si>
+    <t>tengo un par de entregables mas. Lo que me hace ruido es que algunos de mis entregables son las hojas del arbol, y algunas son los nodos. Como seria??</t>
+  </si>
 </sst>
 </file>
 
@@ -158,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +210,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -294,23 +316,24 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -614,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G38"/>
+  <dimension ref="B2:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,24 +653,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -658,7 +681,7 @@
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -677,7 +700,9 @@
         <v>7</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -686,7 +711,9 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -695,7 +722,9 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -704,7 +733,9 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -713,7 +744,9 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -722,7 +755,9 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -731,7 +766,9 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -740,7 +777,9 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -749,7 +788,9 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -758,7 +799,9 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -767,7 +810,9 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -776,7 +821,9 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -785,7 +832,9 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -794,7 +843,9 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -803,7 +854,9 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -812,7 +865,9 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -821,7 +876,9 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -830,7 +887,9 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -839,7 +898,9 @@
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -857,7 +918,9 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -866,7 +929,9 @@
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -875,7 +940,9 @@
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -884,7 +951,9 @@
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -898,7 +967,9 @@
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="E30" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Roles y responsabilidades VS Consistencia
</commit_message>
<xml_diff>
--- a/Documento de consistencia.xlsx
+++ b/Documento de consistencia.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
   <si>
     <t>Documentos</t>
   </si>
@@ -336,7 +336,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Incorrecto" xfId="1" builtinId="27"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -346,12 +346,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -393,7 +396,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -428,7 +431,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -640,10 +643,10 @@
   <dimension ref="B2:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
@@ -699,7 +702,9 @@
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>33</v>
       </c>
@@ -710,7 +715,9 @@
         <v>6</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>34</v>
       </c>
@@ -721,7 +728,9 @@
         <v>3</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>33</v>
       </c>
@@ -732,7 +741,9 @@
         <v>11</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>35</v>
       </c>
@@ -743,7 +754,9 @@
         <v>10</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>33</v>
       </c>
@@ -754,7 +767,9 @@
         <v>9</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>33</v>
       </c>
@@ -765,7 +780,9 @@
         <v>8</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>33</v>
       </c>
@@ -776,7 +793,9 @@
         <v>12</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>33</v>
       </c>
@@ -787,7 +806,9 @@
         <v>23</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>33</v>
       </c>
@@ -798,7 +819,9 @@
         <v>22</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>33</v>
       </c>
@@ -809,7 +832,9 @@
         <v>21</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>33</v>
       </c>
@@ -820,7 +845,9 @@
         <v>20</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>33</v>
       </c>
@@ -831,7 +858,9 @@
         <v>19</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>33</v>
       </c>
@@ -842,7 +871,9 @@
         <v>17</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E18" s="2" t="s">
         <v>34</v>
       </c>
@@ -853,7 +884,9 @@
         <v>18</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E19" s="2" t="s">
         <v>33</v>
       </c>
@@ -864,7 +897,9 @@
         <v>16</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E20" s="2" t="s">
         <v>33</v>
       </c>
@@ -875,7 +910,9 @@
         <v>13</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E21" s="2" t="s">
         <v>33</v>
       </c>
@@ -886,7 +923,9 @@
         <v>14</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E22" s="2" t="s">
         <v>33</v>
       </c>
@@ -897,7 +936,9 @@
         <v>15</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E23" s="2" t="s">
         <v>33</v>
       </c>
@@ -908,7 +949,9 @@
         <v>27</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
@@ -917,7 +960,9 @@
         <v>26</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E25" s="2" t="s">
         <v>33</v>
       </c>
@@ -928,7 +973,9 @@
         <v>4</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E26" s="2" t="s">
         <v>34</v>
       </c>
@@ -939,7 +986,9 @@
         <v>24</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E27" s="2" t="s">
         <v>36</v>
       </c>
@@ -950,7 +999,9 @@
         <v>25</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1044,7 +1095,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1056,7 +1107,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
consistencia acta de proyecto
consistencia acta de proyecto
</commit_message>
<xml_diff>
--- a/Documento de consistencia.xlsx
+++ b/Documento de consistencia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="41">
   <si>
     <t>Documentos</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>tengo un par de entregables mas. Lo que me hace ruido es que algunos de mis entregables son las hojas del arbol, y algunas son los nodos. Como seria??</t>
+  </si>
+  <si>
+    <t>codigo fuente del front end(solo en el WBS va desagregado)</t>
+  </si>
+  <si>
+    <t>script base de datos</t>
+  </si>
+  <si>
+    <t>codigo fuente del back end</t>
   </si>
 </sst>
 </file>
@@ -642,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,6 +711,9 @@
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
@@ -714,7 +726,9 @@
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
@@ -727,7 +741,9 @@
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
@@ -740,7 +756,9 @@
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>33</v>
       </c>
@@ -753,7 +771,9 @@
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>33</v>
       </c>
@@ -766,7 +786,9 @@
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
@@ -779,7 +801,9 @@
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
@@ -792,7 +816,9 @@
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>33</v>
       </c>
@@ -805,7 +831,9 @@
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
@@ -818,7 +846,9 @@
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>33</v>
       </c>
@@ -831,7 +861,9 @@
       <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>33</v>
       </c>
@@ -844,7 +876,9 @@
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>33</v>
       </c>
@@ -857,7 +891,9 @@
       <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>33</v>
       </c>
@@ -870,7 +906,9 @@
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>33</v>
       </c>
@@ -883,7 +921,9 @@
       <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>33</v>
       </c>
@@ -896,7 +936,9 @@
       <c r="B20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>33</v>
       </c>
@@ -909,7 +951,9 @@
       <c r="B21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>33</v>
       </c>
@@ -922,7 +966,9 @@
       <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D22" s="2" t="s">
         <v>33</v>
       </c>
@@ -935,7 +981,9 @@
       <c r="B23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D23" s="2" t="s">
         <v>33</v>
       </c>
@@ -948,7 +996,9 @@
       <c r="B24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>33</v>
       </c>
@@ -959,7 +1009,9 @@
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D25" s="2" t="s">
         <v>33</v>
       </c>
@@ -972,7 +1024,9 @@
       <c r="B26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>33</v>
       </c>
@@ -985,7 +1039,9 @@
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D27" s="2" t="s">
         <v>33</v>
       </c>
@@ -998,7 +1054,9 @@
       <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1024,22 +1082,34 @@
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>

</xml_diff>